<commit_message>
Tender Docuement Preparation Meeting
Tender Docuement Preparation Meeting
</commit_message>
<xml_diff>
--- a/Civilworks cost/Slope Protection/Report Flood Damage.xlsx
+++ b/Civilworks cost/Slope Protection/Report Flood Damage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Stone Shingle(Final)" sheetId="1" r:id="rId1"/>
@@ -530,23 +530,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1064,20 +1064,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>35</v>
       </c>
@@ -1090,7 +1090,7 @@
       <c r="H1" s="40"/>
       <c r="I1" s="40"/>
     </row>
-    <row r="2" spans="1:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -1101,7 +1101,7 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="43" t="s">
         <v>26</v>
       </c>
@@ -1114,7 +1114,7 @@
       <c r="H3" s="43"/>
       <c r="I3" s="43"/>
     </row>
-    <row r="4" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15"/>
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
@@ -1125,7 +1125,7 @@
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="41" t="s">
         <v>34</v>
       </c>
@@ -1138,7 +1138,7 @@
       <c r="H5" s="41"/>
       <c r="I5" s="41"/>
     </row>
-    <row r="7" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="44" t="s">
         <v>16</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="44"/>
       <c r="B8" s="44"/>
       <c r="C8" s="9" t="s">
@@ -1184,7 +1184,7 @@
       <c r="H8" s="42"/>
       <c r="I8" s="44"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A10" s="34">
         <v>1</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>146983173.23623323</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="35">
         <v>2</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>120029450.76009472</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="33">
         <v>3</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>156373464.50947085</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="33">
         <v>4</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>174210343.01885882</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="36">
         <v>5</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>147701755.29790592</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="37">
         <v>6</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>91461856.259265974</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="33">
         <v>7</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>127007159.73255175</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="29"/>
       <c r="B17" s="28" t="s">
         <v>14</v>
@@ -1494,7 +1494,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1504,19 +1504,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>24</v>
       </c>
@@ -1529,33 +1529,33 @@
       <c r="H1" s="40"/>
       <c r="I1" s="40"/>
     </row>
-    <row r="2" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+    <row r="2" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-    </row>
-    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+    </row>
+    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
         <v>16</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="44"/>
       <c r="B6" s="44"/>
       <c r="C6" s="9" t="s">
@@ -1601,7 +1601,7 @@
       <c r="H6" s="42"/>
       <c r="I6" s="44"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>1</v>
       </c>
@@ -1657,7 +1657,7 @@
       </c>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="48">
         <v>2</v>
       </c>
@@ -1680,12 +1680,12 @@
         <f>SUM(C9:F9)</f>
         <v>2.6489999999999996</v>
       </c>
-      <c r="H9" s="46">
+      <c r="H9" s="45">
         <v>1674.9</v>
       </c>
-      <c r="I9" s="47"/>
-    </row>
-    <row r="10" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="I9" s="46"/>
+    </row>
+    <row r="10" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" s="48"/>
       <c r="B10" s="6" t="s">
         <v>20</v>
@@ -1695,10 +1695,10 @@
       <c r="E10" s="48"/>
       <c r="F10" s="48"/>
       <c r="G10" s="49"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="47"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H10" s="45"/>
+      <c r="I10" s="46"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="48"/>
       <c r="B11" s="5" t="s">
         <v>8</v>
@@ -1708,10 +1708,10 @@
       <c r="E11" s="48"/>
       <c r="F11" s="48"/>
       <c r="G11" s="49"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="47"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H11" s="45"/>
+      <c r="I11" s="46"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="48">
         <v>3</v>
       </c>
@@ -1727,18 +1727,18 @@
       <c r="E12" s="48">
         <v>1.155</v>
       </c>
-      <c r="F12" s="47">
+      <c r="F12" s="46">
         <v>0.03</v>
       </c>
       <c r="G12" s="48">
         <v>2.2749999999999999</v>
       </c>
-      <c r="H12" s="46">
+      <c r="H12" s="45">
         <v>1701.95</v>
       </c>
-      <c r="I12" s="47"/>
-    </row>
-    <row r="13" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="I12" s="46"/>
+    </row>
+    <row r="13" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="48"/>
       <c r="B13" s="6" t="s">
         <v>21</v>
@@ -1746,12 +1746,12 @@
       <c r="C13" s="48"/>
       <c r="D13" s="48"/>
       <c r="E13" s="48"/>
-      <c r="F13" s="47"/>
+      <c r="F13" s="46"/>
       <c r="G13" s="48"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="47"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H13" s="45"/>
+      <c r="I13" s="46"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="48"/>
       <c r="B14" s="5" t="s">
         <v>9</v>
@@ -1759,12 +1759,12 @@
       <c r="C14" s="48"/>
       <c r="D14" s="48"/>
       <c r="E14" s="48"/>
-      <c r="F14" s="47"/>
+      <c r="F14" s="46"/>
       <c r="G14" s="48"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="47"/>
-    </row>
-    <row r="15" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="H14" s="45"/>
+      <c r="I14" s="46"/>
+    </row>
+    <row r="15" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A15" s="48">
         <v>4</v>
       </c>
@@ -1774,7 +1774,7 @@
       <c r="C15" s="48">
         <v>1.0940000000000001</v>
       </c>
-      <c r="D15" s="47">
+      <c r="D15" s="46">
         <v>1.097</v>
       </c>
       <c r="E15" s="48">
@@ -1786,38 +1786,38 @@
       <c r="G15" s="48">
         <v>2.1909999999999998</v>
       </c>
-      <c r="H15" s="46">
+      <c r="H15" s="45">
         <v>1036.79</v>
       </c>
-      <c r="I15" s="47"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I15" s="46"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="48"/>
       <c r="B16" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="48"/>
-      <c r="D16" s="47"/>
+      <c r="D16" s="46"/>
       <c r="E16" s="48"/>
       <c r="F16" s="48"/>
       <c r="G16" s="48"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="47"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H16" s="45"/>
+      <c r="I16" s="46"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="48"/>
       <c r="B17" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="48"/>
-      <c r="D17" s="47"/>
+      <c r="D17" s="46"/>
       <c r="E17" s="48"/>
       <c r="F17" s="48"/>
       <c r="G17" s="48"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="47"/>
-    </row>
-    <row r="18" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="H17" s="45"/>
+      <c r="I17" s="46"/>
+    </row>
+    <row r="18" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A18" s="48"/>
       <c r="B18" s="4" t="s">
         <v>22</v>
@@ -1825,7 +1825,7 @@
       <c r="C18" s="48">
         <v>0</v>
       </c>
-      <c r="D18" s="47">
+      <c r="D18" s="46">
         <v>4.8449999999999998</v>
       </c>
       <c r="E18" s="48">
@@ -1838,38 +1838,38 @@
         <f>SUM(C18:F18)</f>
         <v>4.8599999999999994</v>
       </c>
-      <c r="H18" s="46">
+      <c r="H18" s="45">
         <v>1417</v>
       </c>
-      <c r="I18" s="47"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I18" s="46"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="48"/>
       <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="48"/>
-      <c r="D19" s="47"/>
+      <c r="D19" s="46"/>
       <c r="E19" s="48"/>
       <c r="F19" s="48"/>
       <c r="G19" s="49"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="47"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H19" s="45"/>
+      <c r="I19" s="46"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="48"/>
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="48"/>
-      <c r="D20" s="47"/>
+      <c r="D20" s="46"/>
       <c r="E20" s="48"/>
       <c r="F20" s="48"/>
       <c r="G20" s="49"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="47"/>
-    </row>
-    <row r="21" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="H20" s="45"/>
+      <c r="I20" s="46"/>
+    </row>
+    <row r="21" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A21" s="48">
         <v>5</v>
       </c>
@@ -1891,12 +1891,12 @@
       <c r="G21" s="48">
         <v>3.327</v>
       </c>
-      <c r="H21" s="46">
+      <c r="H21" s="45">
         <v>1555.86</v>
       </c>
-      <c r="I21" s="47"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I21" s="46"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="48"/>
       <c r="B22" s="5" t="s">
         <v>13</v>
@@ -1906,10 +1906,10 @@
       <c r="E22" s="48"/>
       <c r="F22" s="48"/>
       <c r="G22" s="48"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="47"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H22" s="45"/>
+      <c r="I22" s="46"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
         <v>14</v>
@@ -1942,6 +1942,38 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="G15:G17"/>
     <mergeCell ref="H21:H22"/>
     <mergeCell ref="I21:I22"/>
     <mergeCell ref="A2:I2"/>
@@ -1958,38 +1990,6 @@
     <mergeCell ref="E18:E20"/>
     <mergeCell ref="F18:F20"/>
     <mergeCell ref="G18:G20"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="I12:I14"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="90" orientation="portrait" r:id="rId1"/>

</xml_diff>